<commit_message>
Launch Feature,Forgot Password Feature,Constants.java,Config properties,testdata file commit
</commit_message>
<xml_diff>
--- a/HerBalanceApp/src/test/resources/test_data/TestData_HerBalance.xlsx
+++ b/HerBalanceApp/src/test/resources/test_data/TestData_HerBalance.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\OneDrive\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEEB97F-25DA-47AC-ADEE-D653147F3ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Program" sheetId="2" r:id="rId2"/>
-    <sheet name="Batch" sheetId="3" r:id="rId3"/>
+    <sheet name="ForgotPassword" sheetId="2" r:id="rId2"/>
+    <sheet name="ResetPassword" sheetId="3" r:id="rId3"/>
     <sheet name="Class" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -23,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>scenarioName</t>
   </si>
@@ -85,39 +79,87 @@
     <t>sdetnumpyninja@gmail.</t>
   </si>
   <si>
-    <t>programName</t>
-  </si>
-  <si>
-    <t>programDescription</t>
-  </si>
-  <si>
-    <t>programStatus</t>
+    <t>email</t>
   </si>
   <si>
     <t>message</t>
   </si>
   <si>
+    <t>Valid Email id</t>
+  </si>
+  <si>
+    <t>validuser@example.com</t>
+  </si>
+  <si>
+    <t>Reset Code Sent</t>
+  </si>
+  <si>
+    <t>Email id without domain</t>
+  </si>
+  <si>
+    <t>user@</t>
+  </si>
+  <si>
+    <t>Please enter a part following '@'. 'user@' is incomplete.</t>
+  </si>
+  <si>
+    <t>Email id without .com</t>
+  </si>
+  <si>
+    <t>user@gmail</t>
+  </si>
+  <si>
+    <t>Please enter a valid email address</t>
+  </si>
+  <si>
+    <t>Email id starts with numeric</t>
+  </si>
+  <si>
+    <t>123user@gmail.com</t>
+  </si>
+  <si>
+    <t>Email id only with special characters</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>A part following '@' should not contain the symbol '#'.</t>
+  </si>
+  <si>
+    <t>Email id starts with .</t>
+  </si>
+  <si>
+    <t>.user@gmail.com</t>
+  </si>
+  <si>
+    <t>Email id ends with .</t>
+  </si>
+  <si>
+    <t>user.@gmail.com</t>
+  </si>
+  <si>
+    <t>Email id blank</t>
+  </si>
+  <si>
+    <t>resetCode</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
     <t>batchName</t>
   </si>
   <si>
+    <t>classTopic</t>
+  </si>
+  <si>
+    <t>classDescription</t>
+  </si>
+  <si>
     <t>noOfClasses</t>
   </si>
   <si>
-    <t>Application Testing</t>
-  </si>
-  <si>
-    <t>SDET</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>classTopic</t>
-  </si>
-  <si>
-    <t>classDescription</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -194,40 +236,19 @@
   </si>
   <si>
     <t>Saranya M</t>
-  </si>
-  <si>
-    <t>Editprogramname</t>
-  </si>
-  <si>
-    <t>sdet165</t>
-  </si>
-  <si>
-    <t>Successfully updated</t>
-  </si>
-  <si>
-    <t>Editprogramdescription</t>
-  </si>
-  <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>VerifyenterProgramandDescriptionname</t>
-  </si>
-  <si>
-    <t>Automation Testing</t>
-  </si>
-  <si>
-    <t>Data Driven</t>
-  </si>
-  <si>
-    <t>CucumberLMSS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -275,10 +296,31 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.9499999999999993"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.95"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -293,14 +335,150 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,8 +491,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -346,49 +710,334 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="48"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -586,12 +1235,11 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -601,14 +1249,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="26.21875" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.2232142857143" customWidth="1"/>
+    <col min="2" max="2" width="25.8839285714286" customWidth="1"/>
+    <col min="3" max="3" width="29.7767857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" customHeight="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +1270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" customHeight="1" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -636,270 +1284,274 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24" customHeight="1">
-      <c r="A3" s="9" t="s">
+    <row r="3" ht="24" customHeight="1" spans="1:5">
+      <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="10" t="s">
+    <row r="4" customHeight="1" spans="1:5">
+      <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A5" s="10" t="s">
+    <row r="5" customHeight="1" spans="1:5">
+      <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A6" s="10" t="s">
+    <row r="6" customHeight="1" spans="1:5">
+      <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A7" s="10" t="s">
+    <row r="7" customHeight="1" spans="1:5">
+      <c r="A7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="13" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" tooltip="mailto:sdetnumpyninja@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C5" r:id="rId2" tooltip="mailto:Feb@2025" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B6" r:id="rId3" tooltip="mailto:sdetnumpyninja@gmail.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C6" r:id="rId4" tooltip="mailto:Feb@2025" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B7" r:id="rId5" tooltip="mailto:sdetnumpyninja@gmail." xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" tooltip="mailto:Feb@2025" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B4" r:id="rId1" display="sdetnumpyninja@gmail.com" tooltip="mailto:sdetnumpyninja@gmail.com"/>
+    <hyperlink ref="C5" r:id="rId2" display="Feb@2025" tooltip="mailto:Feb@2025"/>
+    <hyperlink ref="B6" r:id="rId1" display="sdetnumpyninja@gmail.com" tooltip="mailto:sdetnumpyninja@gmail.com"/>
+    <hyperlink ref="C6" r:id="rId2" display="Feb@2026" tooltip="mailto:Feb@2025"/>
+    <hyperlink ref="B7" r:id="rId3" display="sdetnumpyninja@gmail." tooltip="mailto:sdetnumpyninja@gmail."/>
+    <hyperlink ref="C7" r:id="rId2" display="Feb@2025" tooltip="mailto:Feb@2025"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.7767857142857" customWidth="1"/>
+    <col min="2" max="2" width="27.7767857142857" customWidth="1"/>
+    <col min="3" max="3" width="29.3303571428571" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" customHeight="1" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" customHeight="1" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A9" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C9" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="2:4">
       <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" customHeight="1" spans="2:4">
       <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+    <row r="13" customHeight="1" spans="2:4">
       <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display=".user@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1">
+    <row r="1" customHeight="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -918,29 +1570,14 @@
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-    </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="1">
-        <v>25</v>
-      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -960,10 +1597,8 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1">
+    </row>
+    <row r="3" customHeight="1" spans="1:28">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -993,7 +1628,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1">
+    <row r="4" customHeight="1" spans="1:28">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="7"/>
@@ -1023,7 +1658,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1">
+    <row r="5" customHeight="1" spans="1:28">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1053,7 +1688,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="15.75" customHeight="1">
+    <row r="6" customHeight="1" spans="1:28">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1083,7 +1718,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1">
+    <row r="7" customHeight="1" spans="1:28">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="7"/>
@@ -1115,164 +1750,166 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.8839285714286" customWidth="1"/>
+    <col min="2" max="2" width="18.3303571428571" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="8" max="8" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="30.7767857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12" customHeight="1">
+    <row r="1" ht="12" customHeight="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:9">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:9">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:10">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" tooltip="https://docs.google.com/spreadsheet1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="H5" r:id="rId1" display="https://docs.google.com/spreadsheet1" tooltip="https://docs.google.com/spreadsheet1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merging Login functionality,change in testdata_herbalance.xlsx,part of reset password functionality
</commit_message>
<xml_diff>
--- a/HerBalanceApp/src/test/resources/test_data/TestData_HerBalance.xlsx
+++ b/HerBalanceApp/src/test/resources/test_data/TestData_HerBalance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12040"/>
+    <workbookView windowWidth="28800" windowHeight="12040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,11 +16,113 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>scenarioName</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Static Data</t>
+  </si>
+  <si>
+    <t>Valid Credentials</t>
+  </si>
+  <si>
+    <t>sdet@numpy.com</t>
+  </si>
+  <si>
+    <t>NumpyNinja</t>
+  </si>
+  <si>
+    <t>email without domain name</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Please include an '@' in the email address. 'abc' is missing an '@'.</t>
+  </si>
+  <si>
+    <t>email without .com</t>
+  </si>
+  <si>
+    <t>abc@123</t>
+  </si>
+  <si>
+    <t>Please include '.' in the email address. 'abc.com' is missing an extension.</t>
+  </si>
+  <si>
+    <t>email without @ symbols</t>
+  </si>
+  <si>
+    <t>abc.com</t>
+  </si>
+  <si>
+    <t>Please include an '@' in the email address. 'abc.com' is missing an '@'.</t>
+  </si>
+  <si>
+    <t>email with all numeric values only</t>
+  </si>
+  <si>
+    <t>Please include an '@' in the email address. '1234875' is missing an '@'.</t>
+  </si>
+  <si>
+    <t>email with all special characters only</t>
+  </si>
+  <si>
+    <t>#$#^^#$</t>
+  </si>
+  <si>
+    <t>Please include an '@' in the email address. '#$#^^#$' is missing an '@'.</t>
+  </si>
+  <si>
+    <t>email blank</t>
+  </si>
+  <si>
+    <t>Email is required</t>
+  </si>
+  <si>
+    <t>password field is blank</t>
+  </si>
+  <si>
+    <t>Password is required</t>
+  </si>
+  <si>
+    <t>Invalid Password</t>
+  </si>
+  <si>
+    <t>Cycle synced plans</t>
+  </si>
+  <si>
+    <t>Get nutrition and workout recommendations that align with your hormonal cycle phases</t>
+  </si>
+  <si>
+    <t>Blood work Analysis</t>
+  </si>
+  <si>
+    <t>Upload your lab results for personalized insights on how your health markers impact weight management</t>
+  </si>
+  <si>
+    <t>Personalised Dashboard</t>
+  </si>
+  <si>
+    <t>Track your progress and receive tailored recommendations based on your unique health profile</t>
+  </si>
+  <si>
+    <t>Testimonials</t>
+  </si>
+  <si>
+    <t>"After 3 months with HerBalance, I've lost 18 pounds and finally understand how my cycle affects my weight loss journey!"</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -117,7 +219,7 @@
     <t>Passwords don't match</t>
   </si>
   <si>
-    <t>Submit with weak password</t>
+    <t>Submit with password less than 6 characters</t>
   </si>
   <si>
     <t>pass</t>
@@ -127,6 +229,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Reset code less than </t>
     </r>
     <r>
@@ -153,18 +262,24 @@
   <si>
     <t>Reset code must be 6 digits</t>
   </si>
+  <si>
+    <t>Reset code expired</t>
+  </si>
+  <si>
+    <t>000000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="32">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -177,6 +292,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -220,6 +342,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9.95"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -236,9 +366,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -251,7 +405,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,6 +427,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -274,6 +450,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -281,10 +479,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -296,7 +494,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -305,73 +502,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -385,7 +515,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,187 +530,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,17 +739,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF9A9A9A"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FF9A9A9A"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FF9A9A9A"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color rgb="FF9A9A9A"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -633,24 +778,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -662,6 +789,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -683,26 +836,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -710,160 +846,160 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -872,23 +1008,47 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1150,55 +1310,202 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:E7"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="26.2232142857143" customWidth="1"/>
     <col min="2" max="2" width="25.8839285714286" customWidth="1"/>
     <col min="3" max="3" width="29.7767857142857" customWidth="1"/>
+    <col min="4" max="4" width="38.8303571428571" customWidth="1"/>
+    <col min="5" max="5" width="45.0892857142857" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" customHeight="1" spans="1:5">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:5">
+      <c r="A2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="15"/>
+    </row>
     <row r="3" ht="24" customHeight="1" spans="1:5">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" customHeight="1" spans="1:5">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" customHeight="1" spans="1:5">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" customHeight="1" spans="1:5">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" customHeight="1" spans="1:5">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="A3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:5">
+      <c r="A4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" ht="24" customHeight="1" spans="1:5">
+      <c r="A5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" ht="27" customHeight="1" spans="1:5">
+      <c r="A6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="22">
+        <v>1234875</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" ht="24.5" customHeight="1" spans="1:5">
+      <c r="A7" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:5">
+      <c r="A8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:5">
+      <c r="A9" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" customHeight="1" spans="1:5">
+      <c r="A10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="25">
+        <v>54</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" ht="35" customHeight="1" spans="1:5">
+      <c r="A11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" ht="39.5" customHeight="1" spans="1:5">
+      <c r="A12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" ht="38.5" customHeight="1" spans="1:5">
+      <c r="A13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" ht="40.5" customHeight="1" spans="1:5">
+      <c r="A14" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="abc@123"/>
+    <hyperlink ref="B2" r:id="rId2" display="sdet@numpy.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1228,112 +1535,112 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
+      <c r="A2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
+      <c r="A3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
+      <c r="A4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
+      <c r="A6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>11</v>
+      <c r="A7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>11</v>
+      <c r="A8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="9" t="s">
-        <v>11</v>
+      <c r="A9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="2:4">
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" customHeight="1" spans="2:4">
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="13" customHeight="1" spans="2:4">
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1352,8 +1659,8 @@
   </sheetPr>
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6"/>
@@ -1366,16 +1673,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1401,7 +1708,7 @@
     </row>
     <row r="2" customHeight="1" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1430,19 +1737,19 @@
     </row>
     <row r="3" customHeight="1" spans="1:29">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1">
         <v>123456</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
@@ -1471,19 +1778,19 @@
     </row>
     <row r="4" customHeight="1" spans="1:29">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1">
         <v>123456</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>32</v>
+        <v>65</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="3"/>
@@ -1512,19 +1819,19 @@
     </row>
     <row r="5" customHeight="1" spans="1:29">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1">
         <v>123457</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="3"/>
@@ -1553,19 +1860,19 @@
     </row>
     <row r="6" customHeight="1" spans="1:29">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1">
         <v>12345</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>37</v>
+        <v>61</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="3"/>
@@ -1593,11 +1900,21 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" customHeight="1" spans="1:29">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="3"/>
       <c r="H7" s="1"/>

</xml_diff>

<commit_message>
Reset Password all UI validation functionality without reset user password successfully scenario as that scenario is not implemented in the UI
</commit_message>
<xml_diff>
--- a/HerBalanceApp/src/test/resources/test_data/TestData_HerBalance.xlsx
+++ b/HerBalanceApp/src/test/resources/test_data/TestData_HerBalance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t>scenarioName</t>
   </si>
@@ -204,7 +204,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>Error</t>
+    <t>Invalid or expired reset token</t>
   </si>
   <si>
     <t>Submit with mismatched passwords</t>
@@ -268,6 +268,12 @@
   <si>
     <t>000000</t>
   </si>
+  <si>
+    <t>Submit with all Valid Inputs</t>
+  </si>
+  <si>
+    <t>Your password has been reset successfully</t>
+  </si>
 </sst>
 </file>
 
@@ -279,7 +285,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -301,8 +307,7 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color rgb="FFEF4343"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -318,12 +323,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -854,152 +853,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1010,15 +1009,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1026,19 +1024,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1326,178 +1324,178 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" ht="24" customHeight="1" spans="1:5">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:5">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" ht="24" customHeight="1" spans="1:5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" ht="27" customHeight="1" spans="1:5">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>1234875</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="18" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" ht="24.5" customHeight="1" spans="1:5">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="18" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="15"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="23" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" customHeight="1" spans="1:5">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="23" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>54</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" ht="35" customHeight="1" spans="1:5">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" ht="39.5" customHeight="1" spans="1:5">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" ht="38.5" customHeight="1" spans="1:5">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" ht="40.5" customHeight="1" spans="1:5">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1559,7 +1557,7 @@
       <c r="B3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1570,7 +1568,7 @@
       <c r="B4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1581,7 +1579,7 @@
       <c r="B5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1592,7 +1590,7 @@
       <c r="B6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1600,10 +1598,10 @@
       <c r="A7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1614,7 +1612,7 @@
       <c r="B8" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1623,24 +1621,24 @@
         <v>55</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="2:4">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" customHeight="1" spans="2:4">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="13" customHeight="1" spans="2:4">
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="11"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1657,13 +1655,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="12.6607142857143" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="36.5982142857143" customWidth="1"/>
   </cols>
@@ -1748,7 +1746,7 @@
       <c r="D3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="1"/>
@@ -1903,7 +1901,7 @@
       <c r="A7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1912,7 +1910,7 @@
       <c r="D7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F7" s="1"/>
@@ -1940,6 +1938,20 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
+    <row r="8" customHeight="1" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>